<commit_message>
Changed method to get dataframe of ordered SCEA protocol ids. Replaced None values with empty string when a protocol is applied to some samples and not others. Also changed how the protocol columns are ordered on a protocol type basis. These changes preserve the correct protocol id order for each protocol type.
</commit_message>
<xml_diff>
--- a/hca2scea-backend/test/golden/210420Combined_ES_review.xlsx
+++ b/hca2scea-backend/test/golden/210420Combined_ES_review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Brokering/PROJECTS - IN PROGRESS/GSE121638 - ImmuneRenalCarcinoma/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ami/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E39B9C7D-F008-624F-A4CD-1493C9458931}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF6BFA4-E59B-A243-894C-422B452E99A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="68800" windowHeight="26760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="1101">
   <si>
     <t>PROJECT LABEL (Required)</t>
   </si>
@@ -2070,9 +2070,6 @@
     <t>sequencing_protocol.protocol_core.protocol_id</t>
   </si>
   <si>
-    <t>SRR8088296_1.fastq.gz</t>
-  </si>
-  <si>
     <t>fastq.gz</t>
   </si>
   <si>
@@ -2082,63 +2079,12 @@
     <t>read1</t>
   </si>
   <si>
-    <t>SRR8088296</t>
-  </si>
-  <si>
     <t>sequencing_protocol_1</t>
   </si>
   <si>
-    <t>SRR8088296_2.fastq.gz</t>
-  </si>
-  <si>
     <t>read2</t>
   </si>
   <si>
-    <t>SRR8088297_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088297</t>
-  </si>
-  <si>
-    <t>SRR8088297_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088298_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088298</t>
-  </si>
-  <si>
-    <t>SRR8088298_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088299_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088299</t>
-  </si>
-  <si>
-    <t>SRR8088299_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088300_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088300</t>
-  </si>
-  <si>
-    <t>SRR8088300_2.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088301_1.fastq.gz</t>
-  </si>
-  <si>
-    <t>SRR8088301</t>
-  </si>
-  <si>
-    <t>SRR8088301_2.fastq.gz</t>
-  </si>
-  <si>
     <t>COLLECTION PROTOCOL NAME</t>
   </si>
   <si>
@@ -3156,9 +3102,6 @@
     <t>gene_expression_prep</t>
   </si>
   <si>
-    <t>tcell_prep</t>
-  </si>
-  <si>
     <t>Viable immune (CD45+ Hoechst−) single-cell suspensions generated from ccRCC tumor samples and blood were FACS sorted on a FACS ARIA sorter (BD Biosciences) for lymphoid and myeloid cells (ratio 3:1).  The cells were sorted into ice-cold 1x PBS + 0.04% non-acetylated bovine-serum albumin (New England BioLabs). Sorted cells were counted and viability as assessed using the MoxiGoII counter (Orflo Technologies). Single cells were re-suspended at 1000 cells/ul with a viability &gt; 90%</t>
   </si>
   <si>
@@ -3171,9 +3114,6 @@
     <t>Illumina HiSeq 4000</t>
   </si>
   <si>
-    <t>Single-cell library preparation was carried out as per the 10× Genomics Chromium Single-Cell 5′ Library and Gel Bead Kit v2 #1000014 (10× Genomics, Pleasanton, CA). Cell suspensions were loaded onto a Chromium Single-Cell Chip along with the reverse transcription (RT) master mix and single-cell 5′ gel beads, aiming for 7500 cells per channel. Following generation of single-cell gel bead-in-emulsions (GEMs), RT was performed using a C1000 Touch Thermal Cycler (Bio-Rad Laboratories, Hercules, CA); 13 cycles were used for cDNA amplification. Amplified cDNA was purified using SPRIselect beads (Beckman Coulter, Lane Cove, NSW, Australia) as per the manufacturer’s recommended parameters. Post-cDNA amplification reaction QC and quantification was performed on the Agilent 2100 Bioanalyzer using the DNA High Sensitivity chip. To obtain TCR repertoire profile, VDJ enrichment was carried out as per the Chromium Single Cell V(D)J Enrichment Kit, Human T cell #1000005 (10× Genomics) using 50ng cDNA.  Sequencing libraries were generated with unique sample indices for each sample and quantified.</t>
-  </si>
-  <si>
     <t>10× Genomics Chromium Single-Cell 5′ Library and Gel Bead Kit v2</t>
   </si>
   <si>
@@ -3186,12 +3126,6 @@
     <t>5 prime tag</t>
   </si>
   <si>
-    <t>Chromium Single Cell V(D)J Enrichment Kit, Human T cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> #1000005</t>
-  </si>
-  <si>
     <t>Libraries were sequenced on an Illumina HiSeq 4000 using a 150-pair-end sequencing kit. Gene expression FASTQ files were aligned to the human genome (GRCh38) using the Cell Ranger v2.2 pipeline, while clonotype sequencing was aligned to the vdj_GRCh38_alts_ensembl genome build provided by the manufacturer.</t>
   </si>
   <si>
@@ -3250,12 +3184,6 @@
   </si>
   <si>
     <t>polyA RNA extract</t>
-  </si>
-  <si>
-    <t>10X TCR enrichment</t>
-  </si>
-  <si>
-    <t>EFO:0010714</t>
   </si>
   <si>
     <t>10X 5' v2 sequencing</t>
@@ -4026,22 +3954,22 @@
     </row>
     <row r="6" spans="1:9" s="3" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>990</v>
+        <v>972</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>980</v>
+        <v>962</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>954</v>
+        <v>936</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>953</v>
+        <v>935</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>952</v>
+        <v>934</v>
       </c>
     </row>
   </sheetData>
@@ -4053,8 +3981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:BG11"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="AF6" sqref="AF6:AH11"/>
+    <sheetView topLeftCell="B1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4855,257 +4783,257 @@
     </row>
     <row r="6" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>1060</v>
+        <v>1038</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1014</v>
+        <v>996</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1034</v>
+        <v>1016</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>1035</v>
+        <v>1017</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>1087</v>
+        <v>1063</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>964</v>
+        <v>946</v>
       </c>
       <c r="G6" s="3">
         <v>9606</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>1093</v>
+        <v>1069</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF6" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG6" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH6" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="7" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>1061</v>
+        <v>1039</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1015</v>
+        <v>997</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1034</v>
+        <v>1016</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>1035</v>
+        <v>1017</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>1088</v>
+        <v>1064</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>962</v>
+        <v>944</v>
       </c>
       <c r="G7" s="3">
         <v>9606</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>1094</v>
+        <v>1070</v>
       </c>
       <c r="AC7" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD7" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE7" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF7" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG7" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH7" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="8" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>1062</v>
+        <v>1040</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>1016</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>1034</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>1035</v>
+        <v>1017</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>1089</v>
+        <v>1065</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>981</v>
+        <v>963</v>
       </c>
       <c r="G8" s="3">
         <v>9606</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>1095</v>
+        <v>1071</v>
       </c>
       <c r="AC8" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD8" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE8" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF8" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG8" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH8" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="9" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>1063</v>
+        <v>1041</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1017</v>
+        <v>999</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>1040</v>
+        <v>1021</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>1090</v>
+        <v>1066</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>960</v>
+        <v>942</v>
       </c>
       <c r="G9" s="3">
         <v>9606</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>1096</v>
+        <v>1072</v>
       </c>
       <c r="AC9" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD9" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE9" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF9" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG9" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH9" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="10" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>1064</v>
+        <v>1042</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1018</v>
+        <v>1000</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>1040</v>
+        <v>1021</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>1091</v>
+        <v>1067</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>958</v>
+        <v>940</v>
       </c>
       <c r="G10" s="3">
         <v>9606</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>1097</v>
+        <v>1073</v>
       </c>
       <c r="AC10" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD10" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE10" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF10" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG10" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH10" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="11" spans="1:59" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>1065</v>
+        <v>1043</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1019</v>
+        <v>1001</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>1040</v>
+        <v>1021</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>1092</v>
+        <v>1068</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>956</v>
+        <v>938</v>
       </c>
       <c r="G11" s="3">
         <v>9606</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>1098</v>
+        <v>1074</v>
       </c>
       <c r="AC11" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AD11" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="AE11" s="3" t="s">
         <v>511</v>
       </c>
       <c r="AF11" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
       <c r="AG11" s="9" t="s">
-        <v>1118</v>
+        <v>1094</v>
       </c>
       <c r="AH11" s="9" t="s">
-        <v>1117</v>
+        <v>1093</v>
       </c>
     </row>
   </sheetData>
@@ -5116,10 +5044,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
-  <dimension ref="A1:AY7"/>
+  <dimension ref="A1:AY6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5171,154 +5099,154 @@
         <v>650</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>777</v>
+        <v>759</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>778</v>
+        <v>760</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>781</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>782</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>784</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>785</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>786</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>788</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>789</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>790</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>792</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>793</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>794</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>796</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>797</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>799</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>800</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>802</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>804</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>808</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>809</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>812</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>817</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>820</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:51" ht="85" customHeight="1" x14ac:dyDescent="0.2">
@@ -5326,34 +5254,34 @@
         <v>443</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>824</v>
+        <v>806</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>828</v>
+        <v>810</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>59</v>
@@ -5362,7 +5290,7 @@
         <v>60</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>829</v>
+        <v>811</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>255</v>
@@ -5410,13 +5338,13 @@
         <v>442</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>830</v>
+        <v>812</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>831</v>
+        <v>813</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>832</v>
+        <v>814</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>437</v>
@@ -5437,19 +5365,19 @@
         <v>442</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>833</v>
+        <v>815</v>
       </c>
       <c r="AN2" s="2" t="s">
-        <v>824</v>
+        <v>806</v>
       </c>
       <c r="AO2" s="2" t="s">
-        <v>825</v>
+        <v>807</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>826</v>
+        <v>808</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>827</v>
+        <v>809</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>255</v>
@@ -5470,10 +5398,10 @@
         <v>60</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>834</v>
+        <v>816</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>835</v>
+        <v>817</v>
       </c>
     </row>
     <row r="3" spans="1:51" ht="82" customHeight="1" x14ac:dyDescent="0.2">
@@ -5483,46 +5411,46 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>716</v>
+        <v>698</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>717</v>
+        <v>699</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>840</v>
+        <v>822</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>841</v>
+        <v>823</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>842</v>
+        <v>824</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>843</v>
+        <v>825</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>845</v>
+        <v>827</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>844</v>
+        <v>826</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>461</v>
@@ -5561,13 +5489,13 @@
         <v>466</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>846</v>
+        <v>828</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>847</v>
+        <v>829</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>848</v>
+        <v>830</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>461</v>
@@ -5588,43 +5516,43 @@
         <v>466</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>776</v>
+        <v>758</v>
       </c>
       <c r="AN3" s="2" t="s">
-        <v>836</v>
+        <v>818</v>
       </c>
       <c r="AO3" s="2" t="s">
-        <v>837</v>
+        <v>819</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>838</v>
+        <v>820</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>839</v>
+        <v>821</v>
       </c>
       <c r="AR3" s="2" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="AS3" s="2" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
       <c r="AT3" s="2" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="AU3" s="2" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="AV3" s="2" t="s">
-        <v>850</v>
+        <v>832</v>
       </c>
       <c r="AW3" s="2" t="s">
-        <v>849</v>
+        <v>831</v>
       </c>
       <c r="AX3" s="2" t="s">
-        <v>851</v>
+        <v>833</v>
       </c>
       <c r="AY3" s="2" t="s">
-        <v>852</v>
+        <v>834</v>
       </c>
     </row>
     <row r="4" spans="1:51" ht="32" hidden="1" x14ac:dyDescent="0.2">
@@ -5632,154 +5560,154 @@
         <v>673</v>
       </c>
       <c r="B4" t="s">
+        <v>835</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="D4" t="s">
+        <v>837</v>
+      </c>
+      <c r="E4" t="s">
+        <v>838</v>
+      </c>
+      <c r="F4" t="s">
+        <v>839</v>
+      </c>
+      <c r="G4" t="s">
+        <v>840</v>
+      </c>
+      <c r="H4" t="s">
+        <v>841</v>
+      </c>
+      <c r="I4" t="s">
+        <v>842</v>
+      </c>
+      <c r="J4" t="s">
+        <v>843</v>
+      </c>
+      <c r="K4" t="s">
+        <v>844</v>
+      </c>
+      <c r="L4" t="s">
+        <v>845</v>
+      </c>
+      <c r="M4" t="s">
+        <v>846</v>
+      </c>
+      <c r="N4" t="s">
+        <v>847</v>
+      </c>
+      <c r="O4" t="s">
+        <v>848</v>
+      </c>
+      <c r="P4" t="s">
+        <v>849</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>850</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="S4" t="s">
+        <v>852</v>
+      </c>
+      <c r="T4" t="s">
         <v>853</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="U4" t="s">
         <v>854</v>
       </c>
-      <c r="D4" t="s">
+      <c r="V4" t="s">
         <v>855</v>
       </c>
-      <c r="E4" t="s">
+      <c r="W4" t="s">
         <v>856</v>
       </c>
-      <c r="F4" t="s">
+      <c r="X4" t="s">
         <v>857</v>
       </c>
-      <c r="G4" t="s">
+      <c r="Y4" t="s">
         <v>858</v>
       </c>
-      <c r="H4" t="s">
+      <c r="Z4" t="s">
         <v>859</v>
       </c>
-      <c r="I4" t="s">
+      <c r="AA4" t="s">
         <v>860</v>
       </c>
-      <c r="J4" t="s">
+      <c r="AB4" t="s">
         <v>861</v>
       </c>
-      <c r="K4" t="s">
+      <c r="AC4" t="s">
         <v>862</v>
       </c>
-      <c r="L4" t="s">
+      <c r="AD4" t="s">
         <v>863</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AE4" t="s">
         <v>864</v>
       </c>
-      <c r="N4" t="s">
+      <c r="AF4" t="s">
         <v>865</v>
       </c>
-      <c r="O4" t="s">
+      <c r="AG4" t="s">
         <v>866</v>
       </c>
-      <c r="P4" t="s">
+      <c r="AH4" t="s">
         <v>867</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="AI4" t="s">
         <v>868</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="AJ4" t="s">
         <v>869</v>
       </c>
-      <c r="S4" t="s">
+      <c r="AK4" t="s">
         <v>870</v>
       </c>
-      <c r="T4" t="s">
+      <c r="AL4" t="s">
         <v>871</v>
       </c>
-      <c r="U4" t="s">
+      <c r="AM4" t="s">
         <v>872</v>
       </c>
-      <c r="V4" t="s">
+      <c r="AN4" t="s">
         <v>873</v>
       </c>
-      <c r="W4" t="s">
+      <c r="AO4" t="s">
         <v>874</v>
       </c>
-      <c r="X4" t="s">
+      <c r="AP4" t="s">
         <v>875</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="AQ4" t="s">
         <v>876</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AR4" t="s">
         <v>877</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AS4" t="s">
         <v>878</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AT4" t="s">
         <v>879</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AU4" t="s">
         <v>880</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AV4" t="s">
         <v>881</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AW4" t="s">
         <v>882</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AX4" t="s">
         <v>883</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AY4" t="s">
         <v>884</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>885</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>886</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>887</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>888</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>889</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>890</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>891</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>892</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>893</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>894</v>
-      </c>
-      <c r="AR4" t="s">
-        <v>895</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>896</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>897</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>898</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>899</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>900</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>901</v>
-      </c>
-      <c r="AY4" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="5" spans="1:51" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -5839,13 +5767,13 @@
     </row>
     <row r="6" spans="1:51" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1036</v>
+        <v>1018</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1045</v>
+        <v>1025</v>
       </c>
       <c r="G6" t="s">
-        <v>1086</v>
+        <v>1062</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -5854,116 +5782,51 @@
         <v>16</v>
       </c>
       <c r="K6" t="s">
-        <v>903</v>
+        <v>885</v>
       </c>
       <c r="L6" t="s">
-        <v>1067</v>
+        <v>1045</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>1068</v>
+        <v>1046</v>
       </c>
       <c r="N6" t="s">
-        <v>904</v>
+        <v>886</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>1071</v>
+        <v>1047</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>1072</v>
+        <v>1048</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>1071</v>
+        <v>1047</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>1043</v>
+        <v>1023</v>
       </c>
       <c r="S6" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1049</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1026</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>887</v>
+      </c>
+      <c r="AF6" t="s">
         <v>1044</v>
       </c>
-      <c r="T6" t="s">
-        <v>1073</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>1046</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>905</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>1066</v>
-      </c>
       <c r="AN6" s="3" t="s">
-        <v>1086</v>
+        <v>1062</v>
       </c>
       <c r="AO6">
         <v>16</v>
       </c>
       <c r="AP6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:51" ht="160" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1042</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>1086</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3">
-        <v>16</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>903</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>1067</v>
-      </c>
-      <c r="M7" s="8" t="s">
-        <v>1068</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>904</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>1069</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>1070</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>1069</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>1047</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>1048</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>1073</v>
-      </c>
-      <c r="AD7" s="3" t="s">
-        <v>1046</v>
-      </c>
-      <c r="AE7" s="3" t="s">
-        <v>905</v>
-      </c>
-      <c r="AF7" s="3" t="s">
-        <v>1066</v>
-      </c>
-      <c r="AN7" s="3" t="s">
-        <v>1086</v>
-      </c>
-      <c r="AO7" s="3">
-        <v>16</v>
-      </c>
-      <c r="AP7" s="3">
         <v>10</v>
       </c>
     </row>
@@ -6003,55 +5866,55 @@
         <v>651</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>906</v>
+        <v>888</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>907</v>
+        <v>889</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>908</v>
+        <v>890</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>909</v>
+        <v>891</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>910</v>
+        <v>892</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>911</v>
+        <v>893</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>912</v>
+        <v>894</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>913</v>
+        <v>895</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>914</v>
+        <v>896</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>915</v>
+        <v>897</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>916</v>
+        <v>898</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>917</v>
+        <v>899</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>918</v>
+        <v>900</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>919</v>
+        <v>901</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="323" customHeight="1" x14ac:dyDescent="0.2">
@@ -6059,22 +5922,22 @@
         <v>443</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>920</v>
+        <v>902</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>59</v>
@@ -6083,10 +5946,10 @@
         <v>60</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>921</v>
+        <v>903</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>922</v>
+        <v>904</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>255</v>
@@ -6098,16 +5961,16 @@
         <v>60</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>923</v>
+        <v>905</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>924</v>
+        <v>906</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>925</v>
+        <v>907</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>926</v>
+        <v>908</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="255" customHeight="1" x14ac:dyDescent="0.2">
@@ -6117,43 +5980,43 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>716</v>
+        <v>698</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>717</v>
+        <v>699</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>927</v>
+        <v>909</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>928</v>
+        <v>910</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>927</v>
+        <v>909</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>929</v>
+        <v>911</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>930</v>
+        <v>912</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>931</v>
+        <v>913</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>932</v>
+        <v>914</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>931</v>
+        <v>913</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>933</v>
+        <v>915</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>934</v>
+        <v>916</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>284</v>
@@ -6167,55 +6030,55 @@
         <v>674</v>
       </c>
       <c r="B4" t="s">
-        <v>935</v>
+        <v>917</v>
       </c>
       <c r="C4" t="s">
-        <v>936</v>
+        <v>918</v>
       </c>
       <c r="D4" t="s">
-        <v>937</v>
+        <v>919</v>
       </c>
       <c r="E4" t="s">
-        <v>938</v>
+        <v>920</v>
       </c>
       <c r="F4" t="s">
-        <v>939</v>
+        <v>921</v>
       </c>
       <c r="G4" t="s">
-        <v>940</v>
+        <v>922</v>
       </c>
       <c r="H4" t="s">
-        <v>941</v>
+        <v>923</v>
       </c>
       <c r="I4" t="s">
-        <v>942</v>
+        <v>924</v>
       </c>
       <c r="J4" t="s">
-        <v>943</v>
+        <v>925</v>
       </c>
       <c r="K4" t="s">
-        <v>944</v>
+        <v>926</v>
       </c>
       <c r="L4" t="s">
-        <v>945</v>
+        <v>927</v>
       </c>
       <c r="M4" t="s">
-        <v>946</v>
+        <v>928</v>
       </c>
       <c r="N4" t="s">
-        <v>947</v>
+        <v>929</v>
       </c>
       <c r="O4" t="s">
-        <v>948</v>
+        <v>930</v>
       </c>
       <c r="P4" t="s">
-        <v>949</v>
+        <v>931</v>
       </c>
       <c r="Q4" t="s">
-        <v>950</v>
+        <v>932</v>
       </c>
       <c r="R4" t="s">
-        <v>951</v>
+        <v>933</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -6242,37 +6105,37 @@
     </row>
     <row r="6" spans="1:18" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1049</v>
+        <v>1027</v>
       </c>
       <c r="G6" t="s">
-        <v>1041</v>
+        <v>1022</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>1120</v>
+        <v>1096</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>1041</v>
+        <v>1022</v>
       </c>
       <c r="K6" t="s">
-        <v>991</v>
+        <v>973</v>
       </c>
       <c r="L6" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>1121</v>
+        <v>1097</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>1050</v>
+        <v>1028</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>1052</v>
+        <v>1030</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>1051</v>
+        <v>1029</v>
       </c>
     </row>
   </sheetData>
@@ -6282,10 +6145,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E29"/>
+    <sheetView tabSelected="1" topLeftCell="J3" workbookViewId="0">
+      <selection activeCell="J17" sqref="A6:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6699,928 +6562,460 @@
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
     </row>
-    <row r="6" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="6" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>961</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="J6" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="AD6" s="3" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>960</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>959</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>945</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>958</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J8" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="H6"/>
-      <c r="J6" t="s">
+      <c r="O8" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>957</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="L6" t="s">
-        <v>1060</v>
-      </c>
-      <c r="M6" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N6" t="s">
-        <v>680</v>
-      </c>
-      <c r="O6" t="s">
+      <c r="J9" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>956</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="AD10" s="3" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="AD6" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>681</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="J11" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="AD11" s="3" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>955</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>676</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D12" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="J12" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="AD12" s="3" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>954</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>953</v>
+      </c>
+      <c r="AD13" s="3" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>677</v>
       </c>
-      <c r="G7" t="s">
-        <v>682</v>
-      </c>
-      <c r="H7"/>
-      <c r="J7" t="s">
+      <c r="J14" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N7" t="s">
-        <v>680</v>
-      </c>
-      <c r="O7" t="s">
+      <c r="J15" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="AD15" s="3" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>677</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>1095</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="AD7" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>683</v>
-      </c>
-      <c r="B8" t="s">
-        <v>676</v>
-      </c>
-      <c r="C8" t="s">
-        <v>677</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="J17" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="H8"/>
-      <c r="J8" t="s">
-        <v>684</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N8" t="s">
-        <v>680</v>
-      </c>
-      <c r="O8" t="s">
-        <v>684</v>
-      </c>
-      <c r="AD8" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>685</v>
-      </c>
-      <c r="B9" t="s">
-        <v>676</v>
-      </c>
-      <c r="C9" t="s">
-        <v>677</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G9" t="s">
-        <v>682</v>
-      </c>
-      <c r="H9"/>
-      <c r="J9" t="s">
-        <v>684</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N9" t="s">
-        <v>680</v>
-      </c>
-      <c r="O9" t="s">
-        <v>684</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>686</v>
-      </c>
-      <c r="B10" t="s">
-        <v>676</v>
-      </c>
-      <c r="C10" t="s">
-        <v>677</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G10" t="s">
-        <v>678</v>
-      </c>
-      <c r="H10"/>
-      <c r="J10" t="s">
-        <v>687</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N10" t="s">
-        <v>680</v>
-      </c>
-      <c r="O10" t="s">
-        <v>687</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>688</v>
-      </c>
-      <c r="B11" t="s">
-        <v>676</v>
-      </c>
-      <c r="C11" t="s">
-        <v>677</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G11" t="s">
-        <v>682</v>
-      </c>
-      <c r="H11"/>
-      <c r="J11" t="s">
-        <v>687</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N11" t="s">
-        <v>680</v>
-      </c>
-      <c r="O11" t="s">
-        <v>687</v>
-      </c>
-      <c r="AD11" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>689</v>
-      </c>
-      <c r="B12" t="s">
-        <v>676</v>
-      </c>
-      <c r="C12" t="s">
-        <v>677</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G12" t="s">
-        <v>678</v>
-      </c>
-      <c r="H12"/>
-      <c r="J12" t="s">
-        <v>690</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N12" t="s">
-        <v>680</v>
-      </c>
-      <c r="O12" t="s">
-        <v>690</v>
-      </c>
-      <c r="AD12" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>691</v>
-      </c>
-      <c r="B13" t="s">
-        <v>676</v>
-      </c>
-      <c r="C13" t="s">
-        <v>677</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G13" t="s">
-        <v>682</v>
-      </c>
-      <c r="H13"/>
-      <c r="J13" t="s">
-        <v>690</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N13" t="s">
-        <v>680</v>
-      </c>
-      <c r="O13" t="s">
-        <v>690</v>
-      </c>
-      <c r="AD13" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>692</v>
-      </c>
-      <c r="B14" t="s">
-        <v>676</v>
-      </c>
-      <c r="C14" t="s">
-        <v>677</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G14" t="s">
-        <v>678</v>
-      </c>
-      <c r="H14"/>
-      <c r="J14" t="s">
-        <v>693</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M14" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N14" t="s">
-        <v>680</v>
-      </c>
-      <c r="O14" t="s">
-        <v>693</v>
-      </c>
-      <c r="AD14" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>694</v>
-      </c>
-      <c r="B15" t="s">
-        <v>676</v>
-      </c>
-      <c r="C15" t="s">
-        <v>677</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G15" t="s">
-        <v>682</v>
-      </c>
-      <c r="H15"/>
-      <c r="J15" t="s">
-        <v>693</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N15" t="s">
-        <v>680</v>
-      </c>
-      <c r="O15" t="s">
-        <v>693</v>
-      </c>
-      <c r="AD15" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>695</v>
-      </c>
-      <c r="B16" t="s">
-        <v>676</v>
-      </c>
-      <c r="C16" t="s">
-        <v>677</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G16" t="s">
-        <v>678</v>
-      </c>
-      <c r="H16"/>
-      <c r="J16" t="s">
-        <v>696</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>1065</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N16" t="s">
-        <v>680</v>
-      </c>
-      <c r="O16" t="s">
-        <v>696</v>
-      </c>
-      <c r="AD16" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>697</v>
-      </c>
-      <c r="B17" t="s">
-        <v>676</v>
-      </c>
-      <c r="C17" t="s">
-        <v>677</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G17" t="s">
-        <v>682</v>
-      </c>
-      <c r="H17"/>
-      <c r="J17" t="s">
-        <v>696</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>1065</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>1037</v>
-      </c>
-      <c r="N17" t="s">
-        <v>680</v>
-      </c>
-      <c r="O17" t="s">
-        <v>696</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>979</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>977</v>
-      </c>
-      <c r="L18" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="M18" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N18" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O18" s="3" t="s">
-        <v>977</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="19" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>978</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>977</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>1060</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N19" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O19" s="3" t="s">
-        <v>977</v>
-      </c>
-      <c r="AD19" s="3" t="s">
-        <v>963</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>976</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>974</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M20" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N20" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O20" s="3" t="s">
-        <v>974</v>
-      </c>
-      <c r="AD20" s="3" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>975</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>974</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>1061</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N21" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O21" s="3" t="s">
-        <v>974</v>
-      </c>
-      <c r="AD21" s="3" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="22" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>983</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="L22" s="3" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M22" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="AD22" s="3" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="23" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>984</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>1062</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N23" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>985</v>
-      </c>
-      <c r="AD23" s="3" t="s">
-        <v>982</v>
-      </c>
-    </row>
-    <row r="24" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>973</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>971</v>
-      </c>
-      <c r="L24" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="M24" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N24" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>971</v>
-      </c>
-      <c r="AD24" s="3" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="25" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>972</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>971</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>1063</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>971</v>
-      </c>
-      <c r="AD25" s="3" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="26" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>970</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>968</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N26" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O26" s="3" t="s">
-        <v>968</v>
-      </c>
-      <c r="AD26" s="3" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="27" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>969</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>968</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>1064</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N27" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O27" s="3" t="s">
-        <v>968</v>
-      </c>
-      <c r="AD27" s="3" t="s">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="28" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
-        <v>967</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>1065</v>
-      </c>
-      <c r="M28" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N28" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O28" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="AD28" s="3" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="29" spans="1:30" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>966</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>676</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>677</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>1119</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>677</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="J29" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>1065</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>1036</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="O29" s="3" t="s">
-        <v>965</v>
-      </c>
-      <c r="AD29" s="3" t="s">
-        <v>955</v>
+      <c r="O17" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="AD17" s="3" t="s">
+        <v>937</v>
       </c>
     </row>
   </sheetData>
@@ -7633,7 +7028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="F2" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -7817,16 +7212,16 @@
         <v>85</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>1107</v>
+        <v>1083</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>1099</v>
+        <v>1075</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>1109</v>
+        <v>1085</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7834,16 +7229,16 @@
         <v>86</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>1100</v>
+        <v>1076</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7851,16 +7246,16 @@
         <v>87</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>1101</v>
+        <v>1077</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7868,16 +7263,16 @@
         <v>88</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>1102</v>
+        <v>1078</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7885,16 +7280,16 @@
         <v>89</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>1102</v>
+        <v>1078</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7902,16 +7297,16 @@
         <v>90</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>1103</v>
+        <v>1079</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7919,16 +7314,16 @@
         <v>91</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>1103</v>
+        <v>1079</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7936,22 +7331,22 @@
         <v>92</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>992</v>
+        <v>974</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>1105</v>
+        <v>1081</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>1104</v>
+        <v>1080</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>1111</v>
+        <v>1087</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>991</v>
+        <v>973</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7959,22 +7354,22 @@
         <v>93</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>993</v>
+        <v>975</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>1103</v>
+        <v>1079</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>991</v>
+        <v>973</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -7982,22 +7377,22 @@
         <v>94</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>994</v>
+        <v>976</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>1106</v>
+        <v>1082</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>1103</v>
+        <v>1079</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>1110</v>
+        <v>1086</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>1108</v>
+        <v>1084</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>991</v>
+        <v>973</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.2">
@@ -8147,7 +7542,7 @@
         <v>118</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>995</v>
+        <v>977</v>
       </c>
     </row>
   </sheetData>
@@ -8228,63 +7623,63 @@
         <v>131</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1112</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>996</v>
+        <v>978</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>997</v>
+        <v>979</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>998</v>
+        <v>980</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>999</v>
+        <v>981</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1003</v>
+        <v>985</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>1000</v>
+        <v>982</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1006</v>
+        <v>988</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>1001</v>
+        <v>983</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1004</v>
+        <v>986</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
-        <v>1002</v>
+        <v>984</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1005</v>
+        <v>987</v>
       </c>
     </row>
   </sheetData>
@@ -9346,10 +8741,10 @@
     </row>
     <row r="6" spans="1:77" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>986</v>
+        <v>968</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>989</v>
+        <v>971</v>
       </c>
       <c r="D6" s="3">
         <v>9606</v>
@@ -9358,45 +8753,45 @@
         <v>511</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>511</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>1053</v>
+        <v>1031</v>
       </c>
       <c r="U6" s="3" t="s">
-        <v>1054</v>
+        <v>1032</v>
       </c>
       <c r="V6" s="3">
         <v>69</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AA6" s="9" t="s">
-        <v>1124</v>
+        <v>1100</v>
       </c>
       <c r="AB6" s="9" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AC6" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
       <c r="AD6" s="9" t="s">
-        <v>1123</v>
+        <v>1099</v>
       </c>
       <c r="AE6" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="7" spans="1:77" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>987</v>
+        <v>969</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>989</v>
+        <v>971</v>
       </c>
       <c r="D7" s="3">
         <v>9606</v>
@@ -9405,45 +8800,45 @@
         <v>511</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>511</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>1053</v>
+        <v>1031</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>1054</v>
+        <v>1032</v>
       </c>
       <c r="V7" s="3">
         <v>74</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AA7" s="9" t="s">
-        <v>1124</v>
+        <v>1100</v>
       </c>
       <c r="AB7" s="9" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AC7" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
       <c r="AD7" s="9" t="s">
-        <v>1123</v>
+        <v>1099</v>
       </c>
       <c r="AE7" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="8" spans="1:77" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>988</v>
+        <v>970</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>989</v>
+        <v>971</v>
       </c>
       <c r="D8" s="3">
         <v>9606</v>
@@ -9452,37 +8847,37 @@
         <v>511</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>511</v>
       </c>
       <c r="T8" s="3" t="s">
-        <v>1053</v>
+        <v>1031</v>
       </c>
       <c r="U8" s="3" t="s">
-        <v>1054</v>
+        <v>1032</v>
       </c>
       <c r="V8" s="3">
         <v>67</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AA8" s="9" t="s">
-        <v>1124</v>
+        <v>1100</v>
       </c>
       <c r="AB8" s="9" t="s">
-        <v>1055</v>
+        <v>1033</v>
       </c>
       <c r="AC8" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
       <c r="AD8" s="9" t="s">
-        <v>1123</v>
+        <v>1099</v>
       </c>
       <c r="AE8" s="9" t="s">
-        <v>1122</v>
+        <v>1098</v>
       </c>
     </row>
   </sheetData>
@@ -9515,46 +8910,46 @@
         <v>420</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>698</v>
+        <v>680</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>699</v>
+        <v>681</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>702</v>
+        <v>684</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>703</v>
+        <v>685</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>704</v>
+        <v>686</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>705</v>
+        <v>687</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>628</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>706</v>
+        <v>688</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>707</v>
+        <v>689</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>708</v>
+        <v>690</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>709</v>
+        <v>691</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="323" customHeight="1" x14ac:dyDescent="0.2">
@@ -9562,19 +8957,19 @@
         <v>443</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>255</v>
@@ -9611,13 +9006,13 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>716</v>
+        <v>698</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>717</v>
+        <v>699</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>308</v>
@@ -9652,46 +9047,46 @@
         <v>510</v>
       </c>
       <c r="B4" t="s">
-        <v>718</v>
+        <v>700</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>719</v>
+        <v>701</v>
       </c>
       <c r="D4" t="s">
-        <v>720</v>
+        <v>702</v>
       </c>
       <c r="E4" t="s">
-        <v>721</v>
+        <v>703</v>
       </c>
       <c r="F4" t="s">
-        <v>722</v>
+        <v>704</v>
       </c>
       <c r="G4" t="s">
-        <v>723</v>
+        <v>705</v>
       </c>
       <c r="H4" t="s">
-        <v>724</v>
+        <v>706</v>
       </c>
       <c r="I4" t="s">
-        <v>725</v>
+        <v>707</v>
       </c>
       <c r="J4" t="s">
-        <v>726</v>
+        <v>708</v>
       </c>
       <c r="K4" t="s">
-        <v>727</v>
+        <v>709</v>
       </c>
       <c r="L4" t="s">
-        <v>728</v>
+        <v>710</v>
       </c>
       <c r="M4" t="s">
-        <v>729</v>
+        <v>711</v>
       </c>
       <c r="N4" t="s">
-        <v>730</v>
+        <v>712</v>
       </c>
       <c r="O4" t="s">
-        <v>731</v>
+        <v>713</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -9715,36 +9110,36 @@
     </row>
     <row r="6" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1009</v>
+        <v>991</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1013</v>
+        <v>995</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1056</v>
+        <v>1034</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1013</v>
+        <v>995</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1009</v>
+        <v>991</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1012</v>
+        <v>994</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1059</v>
+        <v>1037</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1012</v>
+        <v>994</v>
       </c>
     </row>
   </sheetData>
@@ -9756,7 +9151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:BH11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="I2" workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6:Q8"/>
     </sheetView>
   </sheetViews>
@@ -10575,19 +9970,19 @@
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1014</v>
+        <v>996</v>
       </c>
       <c r="B6" t="s">
-        <v>1057</v>
+        <v>1035</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>986</v>
+        <v>968</v>
       </c>
       <c r="D6" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="E6" t="s">
-        <v>1020</v>
+        <v>1002</v>
       </c>
       <c r="F6">
         <v>9606</v>
@@ -10598,19 +9993,19 @@
         <v>511</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N6" t="s">
         <v>511</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>1008</v>
+        <v>990</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="BH6" t="s">
         <v>512</v>
@@ -10618,19 +10013,19 @@
     </row>
     <row r="7" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1015</v>
+        <v>997</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1057</v>
+        <v>1035</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>987</v>
+        <v>969</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="E7" t="s">
-        <v>1021</v>
+        <v>1003</v>
       </c>
       <c r="F7">
         <v>9606</v>
@@ -10641,19 +10036,19 @@
         <v>511</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N7" t="s">
         <v>511</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>1008</v>
+        <v>990</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="BH7" t="s">
         <v>513</v>
@@ -10661,19 +10056,19 @@
     </row>
     <row r="8" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>1016</v>
+        <v>998</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1057</v>
+        <v>1035</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>988</v>
+        <v>970</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1010</v>
+        <v>992</v>
       </c>
       <c r="E8" t="s">
-        <v>1022</v>
+        <v>1004</v>
       </c>
       <c r="F8">
         <v>9606</v>
@@ -10684,19 +10079,19 @@
         <v>511</v>
       </c>
       <c r="M8" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N8" t="s">
         <v>511</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>1008</v>
+        <v>990</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>1115</v>
+        <v>1091</v>
       </c>
       <c r="BH8" t="s">
         <v>514</v>
@@ -10704,19 +10099,19 @@
     </row>
     <row r="9" spans="1:60" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>1017</v>
+        <v>999</v>
       </c>
       <c r="B9" t="s">
-        <v>1058</v>
+        <v>1036</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>986</v>
+        <v>968</v>
       </c>
       <c r="D9" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
       <c r="E9" t="s">
-        <v>1023</v>
+        <v>1005</v>
       </c>
       <c r="F9">
         <v>9606</v>
@@ -10727,19 +10122,19 @@
         <v>511</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N9" t="s">
         <v>511</v>
       </c>
       <c r="O9" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="P9" s="9" t="s">
-        <v>1114</v>
+        <v>1090</v>
       </c>
       <c r="Q9" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="BH9" t="s">
         <v>515</v>
@@ -10747,19 +10142,19 @@
     </row>
     <row r="10" spans="1:60" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>1018</v>
+        <v>1000</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1058</v>
+        <v>1036</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>987</v>
+        <v>969</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
       <c r="E10" t="s">
-        <v>1024</v>
+        <v>1006</v>
       </c>
       <c r="F10">
         <v>9606</v>
@@ -10770,19 +10165,19 @@
         <v>511</v>
       </c>
       <c r="M10" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N10" t="s">
         <v>511</v>
       </c>
       <c r="O10" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="P10" s="9" t="s">
-        <v>1114</v>
+        <v>1090</v>
       </c>
       <c r="Q10" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="BH10" t="s">
         <v>516</v>
@@ -10790,19 +10185,19 @@
     </row>
     <row r="11" spans="1:60" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>1019</v>
+        <v>1001</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1058</v>
+        <v>1036</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>988</v>
+        <v>970</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>1011</v>
+        <v>993</v>
       </c>
       <c r="E11" t="s">
-        <v>1025</v>
+        <v>1007</v>
       </c>
       <c r="F11">
         <v>9606</v>
@@ -10813,19 +10208,19 @@
         <v>511</v>
       </c>
       <c r="M11" s="3" t="s">
-        <v>1007</v>
+        <v>989</v>
       </c>
       <c r="N11" t="s">
         <v>511</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>1114</v>
+        <v>1090</v>
       </c>
       <c r="Q11" s="9" t="s">
-        <v>1113</v>
+        <v>1089</v>
       </c>
       <c r="BH11" t="s">
         <v>517</v>
@@ -10841,7 +10236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -10862,46 +10257,46 @@
         <v>545</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>732</v>
+        <v>714</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>733</v>
+        <v>715</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>734</v>
+        <v>716</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>735</v>
+        <v>717</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>736</v>
+        <v>718</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>705</v>
+        <v>687</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>628</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>706</v>
+        <v>688</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>707</v>
+        <v>689</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>708</v>
+        <v>690</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>709</v>
+        <v>691</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="323" customHeight="1" x14ac:dyDescent="0.2">
@@ -10909,19 +10304,19 @@
         <v>443</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>255</v>
@@ -10958,13 +10353,13 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>716</v>
+        <v>698</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>717</v>
+        <v>699</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>308</v>
@@ -10999,46 +10394,46 @@
         <v>626</v>
       </c>
       <c r="B4" t="s">
-        <v>737</v>
+        <v>719</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>738</v>
+        <v>720</v>
       </c>
       <c r="D4" t="s">
-        <v>739</v>
+        <v>721</v>
       </c>
       <c r="E4" t="s">
-        <v>740</v>
+        <v>722</v>
       </c>
       <c r="F4" t="s">
-        <v>741</v>
+        <v>723</v>
       </c>
       <c r="G4" t="s">
-        <v>742</v>
+        <v>724</v>
       </c>
       <c r="H4" t="s">
-        <v>743</v>
+        <v>725</v>
       </c>
       <c r="I4" t="s">
-        <v>744</v>
+        <v>726</v>
       </c>
       <c r="J4" t="s">
-        <v>745</v>
+        <v>727</v>
       </c>
       <c r="K4" t="s">
-        <v>746</v>
+        <v>728</v>
       </c>
       <c r="L4" t="s">
-        <v>747</v>
+        <v>729</v>
       </c>
       <c r="M4" t="s">
-        <v>748</v>
+        <v>730</v>
       </c>
       <c r="N4" t="s">
-        <v>749</v>
+        <v>731</v>
       </c>
       <c r="O4" t="s">
-        <v>750</v>
+        <v>732</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -11062,39 +10457,39 @@
     </row>
     <row r="6" spans="1:15" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>1026</v>
+        <v>1008</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1083</v>
+        <v>1059</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1028</v>
+        <v>1010</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1081</v>
+        <v>1057</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1028</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>1027</v>
+        <v>1009</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1085</v>
+        <v>1061</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1082</v>
+        <v>1058</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1029</v>
+        <v>1011</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>1084</v>
+        <v>1060</v>
       </c>
     </row>
   </sheetData>
@@ -11106,7 +10501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C2" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -11126,37 +10521,37 @@
         <v>546</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>751</v>
+        <v>733</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>752</v>
+        <v>734</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>97</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>700</v>
+        <v>682</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>701</v>
+        <v>683</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>753</v>
+        <v>735</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>754</v>
+        <v>736</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>755</v>
+        <v>737</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>756</v>
+        <v>738</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>757</v>
+        <v>739</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>758</v>
+        <v>740</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="323" customHeight="1" x14ac:dyDescent="0.2">
@@ -11164,19 +10559,19 @@
         <v>443</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>710</v>
+        <v>692</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>711</v>
+        <v>693</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>712</v>
+        <v>694</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>713</v>
+        <v>695</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>714</v>
+        <v>696</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>255</v>
@@ -11188,13 +10583,13 @@
         <v>60</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>759</v>
+        <v>741</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>760</v>
+        <v>742</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>761</v>
+        <v>743</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.2">
@@ -11204,13 +10599,13 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>715</v>
+        <v>697</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>716</v>
+        <v>698</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>717</v>
+        <v>699</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>308</v>
@@ -11222,13 +10617,13 @@
         <v>308</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>762</v>
+        <v>744</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>763</v>
+        <v>745</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>764</v>
+        <v>746</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -11236,37 +10631,37 @@
         <v>627</v>
       </c>
       <c r="B4" t="s">
-        <v>765</v>
+        <v>747</v>
       </c>
       <c r="C4" t="s">
-        <v>766</v>
+        <v>748</v>
       </c>
       <c r="D4" t="s">
-        <v>767</v>
+        <v>749</v>
       </c>
       <c r="E4" t="s">
-        <v>768</v>
+        <v>750</v>
       </c>
       <c r="F4" t="s">
-        <v>769</v>
+        <v>751</v>
       </c>
       <c r="G4" t="s">
-        <v>770</v>
+        <v>752</v>
       </c>
       <c r="H4" t="s">
-        <v>771</v>
+        <v>753</v>
       </c>
       <c r="I4" t="s">
-        <v>772</v>
+        <v>754</v>
       </c>
       <c r="J4" t="s">
-        <v>773</v>
+        <v>755</v>
       </c>
       <c r="K4" t="s">
-        <v>774</v>
+        <v>756</v>
       </c>
       <c r="L4" t="s">
-        <v>775</v>
+        <v>757</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -11287,56 +10682,56 @@
     </row>
     <row r="6" spans="1:12" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>1033</v>
+        <v>1015</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1032</v>
+        <v>1014</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1076</v>
+        <v>1052</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1074</v>
+        <v>1050</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>1075</v>
+        <v>1051</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>1030</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="112" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>1031</v>
+        <v>1013</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1038</v>
+        <v>1019</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1078</v>
+        <v>1054</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>1077</v>
+        <v>1053</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>1078</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>1039</v>
+        <v>1020</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>1116</v>
+        <v>1092</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1079</v>
+        <v>1055</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>1080</v>
+        <v>1056</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>1079</v>
+        <v>1055</v>
       </c>
     </row>
   </sheetData>

</xml_diff>